<commit_message>
Migration to JSR305 annotations
</commit_message>
<xml_diff>
--- a/testdata/TestSheet.xlsx
+++ b/testdata/TestSheet.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -48,6 +48,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -397,8 +398,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Fixed some stuff to make it runnable
</commit_message>
<xml_diff>
--- a/testdata/TestSheet.xlsx
+++ b/testdata/TestSheet.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42ABF5EC-E7C4-4A2E-BD15-412AD77A917E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63E1C270-7424-4392-825D-DD3465F8BF1B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="V100" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -48,7 +42,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -393,13 +386,13 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="5.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -441,8 +434,8 @@
         <v>3</v>
       </c>
       <c r="C5" s="2">
-        <f>$B$4</f>
-        <v>2</v>
+        <f>$B$5</f>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -450,7 +443,7 @@
       <c r="B6" s="1"/>
       <c r="C6" s="3">
         <f>SUM(C3:C5)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add reading of dataset for test
</commit_message>
<xml_diff>
--- a/testdata/TestSheet.xlsx
+++ b/testdata/TestSheet.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -42,6 +42,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -391,8 +392,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="5.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>